<commit_message>
[Github Action: main]: Adding excel lineage report
</commit_message>
<xml_diff>
--- a/output/lineage_customer_orders_demo.xlsx
+++ b/output/lineage_customer_orders_demo.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -684,7 +684,7 @@
       <c r="E9" s="2" t="inlineStr">
         <is>
           <t>datediff(current_date(), CAST(account_open_date AS DATE))
-(first(account_length_days) + 101)</t>
+first(account_length_days)</t>
         </is>
       </c>
     </row>
@@ -1331,10 +1331,91 @@
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>spark_catalog</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>prophecy_demos</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>report_table</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>full_name</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>full_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>spark_catalog</t>
+        </is>
+      </c>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>prophecy_demos</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="inlineStr">
+        <is>
+          <t>report_table</t>
+        </is>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>last_name</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>last_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>spark_catalog</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>prophecy_demos</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>report_table</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
           <t>orders</t>
         </is>
       </c>
-      <c r="E33" s="2" t="inlineStr">
+      <c r="E36" s="2" t="inlineStr">
         <is>
           <t>orders</t>
         </is>

</xml_diff>